<commit_message>
Add ASP.NET Core Web TuyenSinhTBD.Web
</commit_message>
<xml_diff>
--- a/Documents/Estimation - tuyen sinh DH TBD.xlsx
+++ b/Documents/Estimation - tuyen sinh DH TBD.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\light\OneDrive\Documents\GitHub\PhanMemXetTuyen_TBDUni\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F0ED190-CA30-4EF3-B8AD-FB5E087FEF4B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7E8CE36-EA44-4810-A2FD-D9087439819D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -265,7 +265,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -293,12 +293,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -580,12 +574,66 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="7" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="7" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="7" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -595,6 +643,12 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="11" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -604,9 +658,7 @@
     <xf numFmtId="0" fontId="4" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -616,75 +668,17 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="7" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="7" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -968,8 +962,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E1009"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E26" sqref="E26"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -982,23 +976,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="44" t="s">
+      <c r="A1" s="64" t="s">
         <v>22</v>
       </c>
-      <c r="B1" s="45"/>
-      <c r="C1" s="45"/>
-      <c r="D1" s="45"/>
-      <c r="E1" s="45"/>
+      <c r="B1" s="65"/>
+      <c r="C1" s="65"/>
+      <c r="D1" s="65"/>
+      <c r="E1" s="65"/>
     </row>
     <row r="2" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
       <c r="B2" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="46" t="s">
+      <c r="C2" s="66" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="47"/>
+      <c r="D2" s="67"/>
       <c r="E2" s="3"/>
     </row>
     <row r="3" spans="1:5" ht="15" x14ac:dyDescent="0.25">
@@ -1019,13 +1013,13 @@
       </c>
     </row>
     <row r="4" spans="1:5" ht="15" x14ac:dyDescent="0.25">
-      <c r="A4" s="48" t="s">
+      <c r="A4" s="68" t="s">
         <v>7</v>
       </c>
-      <c r="B4" s="38"/>
-      <c r="C4" s="38"/>
-      <c r="D4" s="38"/>
-      <c r="E4" s="47"/>
+      <c r="B4" s="69"/>
+      <c r="C4" s="69"/>
+      <c r="D4" s="69"/>
+      <c r="E4" s="67"/>
     </row>
     <row r="5" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A5" s="5">
@@ -1086,19 +1080,19 @@
       <c r="E9" s="3"/>
     </row>
     <row r="10" spans="1:5" ht="15" x14ac:dyDescent="0.2">
-      <c r="A10" s="49" t="s">
+      <c r="A10" s="60" t="s">
         <v>27</v>
       </c>
-      <c r="B10" s="39"/>
-      <c r="C10" s="38"/>
-      <c r="D10" s="38"/>
-      <c r="E10" s="47"/>
+      <c r="B10" s="61"/>
+      <c r="C10" s="69"/>
+      <c r="D10" s="69"/>
+      <c r="E10" s="67"/>
     </row>
     <row r="11" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A11" s="50">
+      <c r="A11" s="70">
         <v>1</v>
       </c>
-      <c r="B11" s="41" t="s">
+      <c r="B11" s="57" t="s">
         <v>23</v>
       </c>
       <c r="C11" s="31" t="s">
@@ -1112,21 +1106,21 @@
       </c>
     </row>
     <row r="12" spans="1:5" s="35" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A12" s="51"/>
-      <c r="B12" s="42"/>
+      <c r="A12" s="71"/>
+      <c r="B12" s="58"/>
       <c r="C12" s="31" t="s">
         <v>31</v>
       </c>
       <c r="D12" s="13">
         <v>6</v>
       </c>
-      <c r="E12" s="53" t="s">
+      <c r="E12" s="37" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="13" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A13" s="51"/>
-      <c r="B13" s="42"/>
+      <c r="A13" s="71"/>
+      <c r="B13" s="58"/>
       <c r="C13" s="31" t="s">
         <v>29</v>
       </c>
@@ -1136,22 +1130,22 @@
       <c r="E13" s="25"/>
     </row>
     <row r="14" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A14" s="51"/>
-      <c r="B14" s="42"/>
+      <c r="A14" s="71"/>
+      <c r="B14" s="58"/>
       <c r="C14" s="32" t="s">
         <v>35</v>
       </c>
       <c r="D14" s="24">
         <v>24</v>
       </c>
-      <c r="E14" s="54" t="s">
+      <c r="E14" s="38" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="15" spans="1:5" s="19" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A15" s="51"/>
-      <c r="B15" s="42"/>
-      <c r="C15" s="55" t="s">
+      <c r="A15" s="71"/>
+      <c r="B15" s="58"/>
+      <c r="C15" s="39" t="s">
         <v>36</v>
       </c>
       <c r="D15" s="24">
@@ -1160,8 +1154,8 @@
       <c r="E15" s="26"/>
     </row>
     <row r="16" spans="1:5" s="34" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="51"/>
-      <c r="B16" s="42"/>
+      <c r="A16" s="71"/>
+      <c r="B16" s="58"/>
       <c r="C16" s="32" t="s">
         <v>38</v>
       </c>
@@ -1171,22 +1165,22 @@
       <c r="E16" s="26"/>
     </row>
     <row r="17" spans="1:5" s="35" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="51"/>
-      <c r="B17" s="42"/>
+      <c r="A17" s="71"/>
+      <c r="B17" s="58"/>
       <c r="C17" s="32" t="s">
         <v>37</v>
       </c>
       <c r="D17" s="24">
         <v>6</v>
       </c>
-      <c r="E17" s="58" t="s">
+      <c r="E17" s="42" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="18" spans="1:5" s="35" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="51"/>
-      <c r="B18" s="42"/>
-      <c r="C18" s="57" t="s">
+      <c r="A18" s="71"/>
+      <c r="B18" s="58"/>
+      <c r="C18" s="41" t="s">
         <v>39</v>
       </c>
       <c r="D18" s="24">
@@ -1195,9 +1189,9 @@
       <c r="E18" s="26"/>
     </row>
     <row r="19" spans="1:5" s="35" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="51"/>
-      <c r="B19" s="42"/>
-      <c r="C19" s="56" t="s">
+      <c r="A19" s="71"/>
+      <c r="B19" s="58"/>
+      <c r="C19" s="40" t="s">
         <v>41</v>
       </c>
       <c r="D19" s="24">
@@ -1206,9 +1200,9 @@
       <c r="E19" s="26"/>
     </row>
     <row r="20" spans="1:5" s="34" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="52"/>
-      <c r="B20" s="43"/>
-      <c r="C20" s="56" t="s">
+      <c r="A20" s="72"/>
+      <c r="B20" s="59"/>
+      <c r="C20" s="40" t="s">
         <v>40</v>
       </c>
       <c r="D20" s="24">
@@ -1217,34 +1211,34 @@
       <c r="E20" s="26"/>
     </row>
     <row r="21" spans="1:5" s="35" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="49" t="s">
+      <c r="A21" s="60" t="s">
         <v>28</v>
       </c>
-      <c r="B21" s="39"/>
-      <c r="C21" s="63"/>
-      <c r="D21" s="39"/>
-      <c r="E21" s="40"/>
+      <c r="B21" s="61"/>
+      <c r="C21" s="62"/>
+      <c r="D21" s="61"/>
+      <c r="E21" s="63"/>
     </row>
     <row r="22" spans="1:5" s="35" customFormat="1" ht="99" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="64">
+      <c r="A22" s="45">
         <v>1</v>
       </c>
-      <c r="B22" s="65" t="s">
+      <c r="B22" s="46" t="s">
         <v>25</v>
       </c>
-      <c r="C22" s="71"/>
+      <c r="C22" s="51"/>
       <c r="D22" s="24">
         <v>56</v>
       </c>
-      <c r="E22" s="72" t="s">
+      <c r="E22" s="52" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="23" spans="1:5" s="35" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="64">
+      <c r="A23" s="45">
         <v>3</v>
       </c>
-      <c r="B23" s="65" t="s">
+      <c r="B23" s="46" t="s">
         <v>44</v>
       </c>
       <c r="C23" s="32" t="s">
@@ -1253,59 +1247,59 @@
       <c r="D23" s="24">
         <v>16</v>
       </c>
-      <c r="E23" s="61" t="s">
+      <c r="E23" s="44" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="24" spans="1:5" s="19" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="74">
+      <c r="A24" s="54">
         <v>5</v>
       </c>
-      <c r="B24" s="41" t="s">
+      <c r="B24" s="57" t="s">
         <v>26</v>
       </c>
-      <c r="C24" s="67" t="s">
+      <c r="C24" s="74" t="s">
         <v>21</v>
       </c>
-      <c r="D24" s="59"/>
-      <c r="E24" s="62" t="s">
+      <c r="D24" s="75"/>
+      <c r="E24" s="76" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="25" spans="1:5" s="35" customFormat="1" ht="42.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="75"/>
-      <c r="B25" s="42"/>
-      <c r="C25" s="68" t="s">
+      <c r="A25" s="55"/>
+      <c r="B25" s="58"/>
+      <c r="C25" s="48" t="s">
         <v>50</v>
       </c>
-      <c r="D25" s="73">
+      <c r="D25" s="53">
         <v>16</v>
       </c>
-      <c r="E25" s="66" t="s">
+      <c r="E25" s="47" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="26" spans="1:5" s="35" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="75"/>
-      <c r="B26" s="42"/>
-      <c r="C26" s="69" t="s">
+      <c r="A26" s="55"/>
+      <c r="B26" s="58"/>
+      <c r="C26" s="49" t="s">
         <v>46</v>
       </c>
       <c r="D26" s="24">
         <v>12</v>
       </c>
-      <c r="E26" s="70"/>
+      <c r="E26" s="50"/>
     </row>
     <row r="27" spans="1:5" s="35" customFormat="1" ht="59.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="76"/>
-      <c r="B27" s="43"/>
-      <c r="C27" s="69" t="s">
+      <c r="A27" s="56"/>
+      <c r="B27" s="59"/>
+      <c r="C27" s="49" t="s">
         <v>47</v>
       </c>
       <c r="D27" s="24">
         <v>12</v>
       </c>
-      <c r="E27" s="60" t="s">
+      <c r="E27" s="43" t="s">
         <v>45</v>
       </c>
     </row>
@@ -1325,7 +1319,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C30" s="16" t="s">
         <v>13</v>
       </c>
@@ -1356,13 +1350,13 @@
       <c r="D33" s="15"/>
     </row>
     <row r="34" spans="1:5" ht="15" x14ac:dyDescent="0.2">
-      <c r="A34" s="37" t="s">
+      <c r="A34" s="73" t="s">
         <v>19</v>
       </c>
-      <c r="B34" s="38"/>
-      <c r="C34" s="38"/>
-      <c r="D34" s="39"/>
-      <c r="E34" s="40"/>
+      <c r="B34" s="69"/>
+      <c r="C34" s="69"/>
+      <c r="D34" s="61"/>
+      <c r="E34" s="63"/>
     </row>
     <row r="35" spans="1:5" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A35" s="3"/>
@@ -4284,6 +4278,7 @@
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="A34:E34"/>
     <mergeCell ref="A24:A27"/>
     <mergeCell ref="B24:B27"/>
     <mergeCell ref="A21:E21"/>
@@ -4293,7 +4288,6 @@
     <mergeCell ref="A10:E10"/>
     <mergeCell ref="A11:A20"/>
     <mergeCell ref="B11:B20"/>
-    <mergeCell ref="A34:E34"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>